<commit_message>
Add ACLCrossCheckTask reports for 20251129
</commit_message>
<xml_diff>
--- a/v12/LOG/ACLCrossCheckTask/20251129-同平台N9K ACL检查.xlsx
+++ b/v12/LOG/ACLCrossCheckTask/20251129-同平台N9K ACL检查.xlsx
@@ -24,16 +24,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,9 +53,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -424,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A684"/>
+  <dimension ref="A1:B627"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,12 +429,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX00-CS01-N9K-TWIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX00-CS01-N9K-TWIDC.log</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>20251129-HX00-OOB-DS01-C3850-TWIDC.log</t>
         </is>
       </c>
     </row>
@@ -448,6 +450,11 @@
           <t>ip access-list VLAN100-ACL</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN15-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -455,6 +462,11 @@
           <t>162 permit tcp 10.10.100.31/32 eq 55888 10.10.108.63/32</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.15.0 0.0.0.255 eq www 443 5480 5900 10.10.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -462,6 +474,11 @@
           <t>164 permit tcp 10.10.100.32/30 eq 55888 10.10.108.63/32</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.150.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -469,6 +486,11 @@
           <t>166 permit tcp 10.10.100.31/32 eq 50051 10.10.106.21/28</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>permit udp 10.10.15.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -476,6 +498,11 @@
           <t>168 permit tcp 10.10.100.32/30 eq 50051 10.10.106.21/28</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>permit udp 10.10.150.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -483,6 +510,11 @@
           <t>170 permit tcp 10.10.100.31/32 10.10.26.41/32 eq 8080</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.150.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -490,6 +522,11 @@
           <t>172 permit tcp 10.10.100.32/30 10.10.26.41/32 eq 8080</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.231 10.10.150.0 0.0.0.255 eq www 443 log</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -497,6 +534,11 @@
           <t>176 permit tcp 10.10.100.31/32 10.10.62.104/30 eq 9092</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.231 10.10.151.0 0.0.0.255 eq www 443 log</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -504,6 +546,18 @@
           <t>178 permit tcp 10.10.100.32/30 10.10.62.104/30 eq 9092</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.231 10.10.152.0 0.0.0.255 eq www 443 log</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.231 10.10.153.0 0.0.0.255 eq www 443 log</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -511,6 +565,11 @@
           <t>ip access-list VLAN106-ACL</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.231 10.10.86.0 0.0.0.255 eq www 443 log</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -518,6 +577,11 @@
           <t>60 permit tcp 10.10.106.0/24 eq 55888 10.10.108.63/32</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.230 eq 3389 host 10.10.80.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -525,6 +589,11 @@
           <t>98 permit tcp 10.10.106.48/28 10.10.62.104/30 eq 9092</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.233 eq 22 host 10.10.108.60 log</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -532,6 +601,11 @@
           <t>100 permit tcp 10.10.106.48/28 10.10.62.104/32 eq 9092</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.15.234 eq 22 host 10.10.108.60 log</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -546,6 +620,11 @@
           <t>158 permit ip 10.10.106.0/27 10.10.26.0/30</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN151-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -553,6 +632,11 @@
           <t>160 permit tcp 10.10.106.40/27 10.10.26.70/31 eq 30080</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.151.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -560,6 +644,11 @@
           <t>162 permit tcp 10.10.106.40/27 10.10.26.70/31 eq 30443</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>permit udp 10.10.151.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -567,6 +656,11 @@
           <t>164 permit tcp 10.10.106.51/28 eq www 10.10.26.1/30</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.151.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -581,6 +675,11 @@
           <t>168 permit tcp 10.10.106.1/29 eq 13080 10.10.26.1/30</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN152-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -588,6 +687,11 @@
           <t>170 permit tcp 10.10.106.1/29 eq 33080 10.10.26.1/30</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.152.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -595,6 +699,11 @@
           <t>172 permit ip 10.10.106.14/31 10.10.26.1/30</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>permit udp 10.10.152.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -602,6 +711,11 @@
           <t>176 permit tcp 10.10.106.32/30 eq 8070 10.10.62.88/31</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.152.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -616,6 +730,11 @@
           <t>184 permit ip 10.10.106.0/27 10.10.26.0/30</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN153-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -623,6 +742,11 @@
           <t>186 permit ip 10.10.106.51/28 10.10.26.0/30</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.153.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -630,6 +754,11 @@
           <t>188 permit tcp 10.10.106.16/30 eq www 10.10.26.0/30</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>permit udp 10.10.153.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -637,6 +766,11 @@
           <t>190 permit tcp 10.10.106.16/30 eq www 10.10.26.60/32</t>
         </is>
       </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.153.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -651,6 +785,11 @@
           <t>206 permit tcp 10.10.106.32/30 eq 8080 10.10.26.1/30</t>
         </is>
       </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN80-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -658,6 +797,11 @@
           <t>208 permit tcp 10.10.106.21/28 10.10.100.31/32 eq 50051</t>
         </is>
       </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>permit ip host 10.10.80.26 10.10.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -665,6 +809,11 @@
           <t>210 permit tcp 10.10.106.21/28 10.10.100.32/30 eq 50051</t>
         </is>
       </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.80.1 10.10.88.0 0.0.0.255 eq 22 log</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -672,6 +821,11 @@
           <t>212 permit tcp 10.10.106.40/32 eq 5000 10.10.62.88/31</t>
         </is>
       </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.80.11 10.10.88.0 0.0.0.255 eq 22 log</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -679,6 +833,11 @@
           <t>218 permit tcp 10.10.106.14/31 10.10.128.6/28 eq 30080</t>
         </is>
       </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>permit udp host 10.10.80.2 10.10.88.0 0.0.0.255 eq snmp log</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -686,6 +845,11 @@
           <t>220 permit tcp 10.10.106.14/31 10.10.128.56/29 eq 30080</t>
         </is>
       </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.10.80.1 host 10.10.15.230 eq 3389 log</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -693,6 +857,11 @@
           <t>222 permit tcp 10.10.106.44/30 10.10.128.0/28 eq 30080</t>
         </is>
       </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>permit ip host 10.10.80.28 10.10.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -707,6 +876,11 @@
           <t>226 permit tcp 10.10.106.44/30 10.10.128.56/28 eq 30080</t>
         </is>
       </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN86-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -714,6 +888,11 @@
           <t>228 permit tcp 10.10.106.48/32 10.10.128.56/28 eq 30080</t>
         </is>
       </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.86.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -721,6 +900,11 @@
           <t>230 permit tcp 10.10.106.48/28 10.10.62.104/30 eq 9092</t>
         </is>
       </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.86.0 0.0.0.255 eq 22 host 10.10.80.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -728,6 +912,11 @@
           <t>232 permit tcp 10.10.106.14/31 10.10.62.104/30 eq 9092</t>
         </is>
       </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>permit ip host 10.10.86.101 10.10.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -735,6 +924,11 @@
           <t>238 permit tcp 10.10.106.12/31 10.10.26.70/31 eq 30080</t>
         </is>
       </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>permit ip host 10.10.86.101 host 10.10.88.247 log</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -742,6 +936,11 @@
           <t>256 permit tcp 10.10.106.43/32 eq 9080 10.10.170.1/30</t>
         </is>
       </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>permit ip host 10.10.86.102 10.10.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -756,6 +955,11 @@
           <t>260 permit tcp 10.10.106.43/32 eq 9080 10.10.128.16/28</t>
         </is>
       </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN88-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -763,6 +967,11 @@
           <t>262 permit tcp 10.10.106.43/32 eq 9080 10.10.128.64/28</t>
         </is>
       </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.80.26 log</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -770,6 +979,11 @@
           <t>264 permit tcp 10.10.106.43/32 eq 9080 10.10.62.32/32</t>
         </is>
       </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.88.0 0.0.0.255 eq 22 host 10.10.80.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -777,6 +991,11 @@
           <t>266 permit tcp 10.10.106.43/32 eq 9080 10.10.62.32/31</t>
         </is>
       </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>permit tcp 10.10.88.0 0.0.0.255 eq 22 host 10.10.80.11 log</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -784,6 +1003,11 @@
           <t>284 permit tcp 10.10.106.40/32 range 8001 8002 10.10.62.33/32</t>
         </is>
       </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.86.101 log</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -791,6 +1015,11 @@
           <t>286 permit tcp 10.10.106.1/29 10.10.26.180/32 eq 10000</t>
         </is>
       </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>permit ip host 10.10.88.247 host 10.10.86.101 log</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -798,6 +1027,11 @@
           <t>288 permit tcp 10.10.106.1/29 10.10.180.31/32 eq 10000</t>
         </is>
       </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>permit udp 10.10.88.0 0.0.0.255 eq snmp host 10.10.80.2 log</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -805,6 +1039,11 @@
           <t>290 permit tcp 10.10.106.1/29 10.10.180.32/32 eq 10000</t>
         </is>
       </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.86.102 log</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -812,6 +1051,11 @@
           <t>292 permit tcp 10.10.106.21/32 eq 10000 10.10.128.14/27</t>
         </is>
       </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.80.28 log</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4716,349 +4960,6 @@
       <c r="A627" t="inlineStr">
         <is>
           <t>62 permit tcp 10.10.7.0/24 eq 5480 10.10.62.32/31</t>
-        </is>
-      </c>
-    </row>
-    <row r="630">
-      <c r="A630" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX00-OOB-DS01-C3850-TWIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="631">
-      <c r="A631" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN15-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="632">
-      <c r="A632" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.15.0 0.0.0.255 eq www 443 5480 5900 10.10.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="633">
-      <c r="A633" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.150.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="634">
-      <c r="A634" t="inlineStr">
-        <is>
-          <t>permit udp 10.10.15.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="635">
-      <c r="A635" t="inlineStr">
-        <is>
-          <t>permit udp 10.10.150.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="636">
-      <c r="A636" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.150.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="637">
-      <c r="A637" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.231 10.10.150.0 0.0.0.255 eq www 443 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="638">
-      <c r="A638" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.231 10.10.151.0 0.0.0.255 eq www 443 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="639">
-      <c r="A639" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.231 10.10.152.0 0.0.0.255 eq www 443 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="640">
-      <c r="A640" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.231 10.10.153.0 0.0.0.255 eq www 443 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="641">
-      <c r="A641" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.231 10.10.86.0 0.0.0.255 eq www 443 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="642">
-      <c r="A642" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.230 eq 3389 host 10.10.80.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="643">
-      <c r="A643" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.233 eq 22 host 10.10.108.60 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="644">
-      <c r="A644" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.15.234 eq 22 host 10.10.108.60 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="646">
-      <c r="A646" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN151-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="647">
-      <c r="A647" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.151.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="648">
-      <c r="A648" t="inlineStr">
-        <is>
-          <t>permit udp 10.10.151.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="649">
-      <c r="A649" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.151.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="651">
-      <c r="A651" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN152-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="652">
-      <c r="A652" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.152.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="653">
-      <c r="A653" t="inlineStr">
-        <is>
-          <t>permit udp 10.10.152.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="654">
-      <c r="A654" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.152.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="656">
-      <c r="A656" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN153-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="657">
-      <c r="A657" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.153.0 0.0.0.255 eq www 443 5900 10.10.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="658">
-      <c r="A658" t="inlineStr">
-        <is>
-          <t>permit udp 10.10.153.0 0.0.0.255 eq snmp 10.10.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="659">
-      <c r="A659" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.153.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="661">
-      <c r="A661" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN80-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="662">
-      <c r="A662" t="inlineStr">
-        <is>
-          <t>permit ip host 10.10.80.26 10.10.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="663">
-      <c r="A663" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.80.1 10.10.88.0 0.0.0.255 eq 22 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="664">
-      <c r="A664" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.80.11 10.10.88.0 0.0.0.255 eq 22 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="665">
-      <c r="A665" t="inlineStr">
-        <is>
-          <t>permit udp host 10.10.80.2 10.10.88.0 0.0.0.255 eq snmp log</t>
-        </is>
-      </c>
-    </row>
-    <row r="666">
-      <c r="A666" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.10.80.1 host 10.10.15.230 eq 3389 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="667">
-      <c r="A667" t="inlineStr">
-        <is>
-          <t>permit ip host 10.10.80.28 10.10.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="669">
-      <c r="A669" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN86-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="670">
-      <c r="A670" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.86.0 0.0.0.255 eq www 443 host 10.10.15.231 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="671">
-      <c r="A671" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.86.0 0.0.0.255 eq 22 host 10.10.80.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="672">
-      <c r="A672" t="inlineStr">
-        <is>
-          <t>permit ip host 10.10.86.101 10.10.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="673">
-      <c r="A673" t="inlineStr">
-        <is>
-          <t>permit ip host 10.10.86.101 host 10.10.88.247 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="674">
-      <c r="A674" t="inlineStr">
-        <is>
-          <t>permit ip host 10.10.86.102 10.10.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="676">
-      <c r="A676" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN88-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="677">
-      <c r="A677" t="inlineStr">
-        <is>
-          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.80.26 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="678">
-      <c r="A678" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.88.0 0.0.0.255 eq 22 host 10.10.80.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="679">
-      <c r="A679" t="inlineStr">
-        <is>
-          <t>permit tcp 10.10.88.0 0.0.0.255 eq 22 host 10.10.80.11 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="680">
-      <c r="A680" t="inlineStr">
-        <is>
-          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.86.101 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="681">
-      <c r="A681" t="inlineStr">
-        <is>
-          <t>permit ip host 10.10.88.247 host 10.10.86.101 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="682">
-      <c r="A682" t="inlineStr">
-        <is>
-          <t>permit udp 10.10.88.0 0.0.0.255 eq snmp host 10.10.80.2 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="683">
-      <c r="A683" t="inlineStr">
-        <is>
-          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.86.102 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="684">
-      <c r="A684" t="inlineStr">
-        <is>
-          <t>permit ip 10.10.88.0 0.0.0.255 host 10.10.80.28 log</t>
         </is>
       </c>
     </row>
@@ -5073,7 +4974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A313"/>
+  <dimension ref="A1:B282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5082,12 +4983,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX01-CS01-N9K-TWIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX01-CS01-N9K-TWIDC.log</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>20251129-HX01-OOB-DS01-C3850-TWIDC.log</t>
         </is>
       </c>
     </row>
@@ -5097,6 +5004,11 @@
           <t>ip access-list VLAN108-ACL</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN15-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5104,6 +5016,11 @@
           <t>60 permit tcp 10.6.108.0/24 10.6.62.66/32 eq www log</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>permit udp 10.6.15.0 0.0.0.255 eq snmp 10.6.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -5111,6 +5028,11 @@
           <t>68 permit tcp 10.6.108.0/24 10.6.62.11/32 eq 16000 log</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>permit udp 10.6.150.0 0.0.0.255 eq snmp 10.6.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -5118,6 +5040,11 @@
           <t>280 permit tcp 10.6.108.60/32 10.6.19.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.15.0 0.0.0.255 eq 443 5900 10.6.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5125,6 +5052,11 @@
           <t>282 permit tcp 10.6.108.60/32 10.6.24.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.150.0 0.0.0.255 eq 443 5900 10.6.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5132,6 +5064,11 @@
           <t>284 permit tcp 10.6.108.60/32 10.6.25.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.15.230 0.0.0.1 10.6.150.0 0.0.0.255 eq www 443</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5139,6 +5076,11 @@
           <t>286 permit tcp 10.6.108.60/32 10.6.26.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.150.0 0.0.0.255 eq www 443 10.6.15.230 0.0.0.1</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5153,6 +5095,11 @@
           <t>288 permit tcp 10.6.108.60/32 10.6.28.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN80-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5160,6 +5107,11 @@
           <t>290 permit tcp 10.6.108.60/32 10.6.0.0/16 eq 22</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.80.0 0.0.0.15 10.6.86.0 0.0.0.255 eq 22 www 443 5480 5900 5601 8000 8980 log</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5167,6 +5119,11 @@
           <t>292 permit icmp 10.6.108.60/32 10.6.0.0/16 log</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.80.0 0.0.0.15 host 10.6.88.243 eq 443 log</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -5174,6 +5131,18 @@
           <t>298 permit tcp 10.6.108.0/24 10.6.200.60/32 eq 1000</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.80.0 0.0.0.15 host 10.6.88.221 eq www 8888 log</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.80.0 0.0.0.15 10.6.88.0 0.0.0.255 eq ftp 22 telnet www 443 log</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -5188,6 +5157,11 @@
           <t>16 deny ip 10.6.130.0/24 10.6.16.72/32</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN86-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -5195,6 +5169,11 @@
           <t>17 deny ip 10.6.130.0/24 10.6.16.168/32</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.86.0 0.0.0.255 eq 22 www 443 5480 5900 5601 8000 8980 10.6.80.0 0.0.0.15 log</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -5202,6 +5181,11 @@
           <t>72 permit tcp 10.6.130.0/24 10.6.62.11/32 eq 16000 log</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>permit ip host 10.6.86.32 10.6.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -5209,6 +5193,11 @@
           <t>205 permit tcp 10.6.130.0/24 10.6.25.204/30 eq 9092</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>permit ip host 10.6.86.33 10.6.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -5216,6 +5205,11 @@
           <t>206 permit tcp 10.6.130.0/24 10.6.25.208/32 eq 9092</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>permit ip host 10.6.86.110 10.6.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5223,6 +5217,11 @@
           <t>207 permit tcp 10.6.130.0/24 10.6.25.204/30 eq 9200</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>permit ip host 10.6.86.52 host 10.6.88.222</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5230,6 +5229,11 @@
           <t>208 permit tcp 10.6.130.0/24 10.6.25.208/32 eq 9200</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>permit ip host 10.6.86.62 host 10.6.88.222</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5244,6 +5248,11 @@
           <t>290 permit tcp 10.6.130.0/24 10.6.13.136/29 range 3366 3369</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN88-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5251,6 +5260,11 @@
           <t>296 permit tcp 10.6.130.0/24 10.6.11.0/27 eq 9092</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>permit udp host 10.6.88.222 host 10.6.88.254 eq snmp log</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -5258,6 +5272,11 @@
           <t>298 permit tcp 10.6.130.0/24 10.6.16.0/27 range 4000 9200</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>permit ip 10.6.88.0 0.0.0.255 host 10.6.86.32 log</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5265,6 +5284,11 @@
           <t>310 permit tcp 10.6.130.0/24 10.6.13.137/32 eq 3306</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>permit ip 10.6.88.0 0.0.0.255 host 10.6.86.33 log</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -5272,6 +5296,11 @@
           <t>320 permit tcp 10.6.130.0/24 10.6.27.32/28 eq 9200</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>permit tcp 10.6.88.0 0.0.0.255 eq ftp 22 telnet www 443 10.6.80.0 0.0.0.15 log</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -5279,6 +5308,11 @@
           <t>322 permit tcp 10.6.130.0/24 10.6.27.80/29 eq 9200</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>permit ip 10.6.88.0 0.0.0.255 host 10.6.86.110 log</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -6992,188 +7026,6 @@
       <c r="A282" t="inlineStr">
         <is>
           <t>386 permit tcp 10.6.8.0/24 10.6.200.60/32 eq 1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX01-OOB-DS01-C3850-TWIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN15-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="inlineStr">
-        <is>
-          <t>permit udp 10.6.15.0 0.0.0.255 eq snmp 10.6.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="inlineStr">
-        <is>
-          <t>permit udp 10.6.150.0 0.0.0.255 eq snmp 10.6.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.15.0 0.0.0.255 eq 443 5900 10.6.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.150.0 0.0.0.255 eq 443 5900 10.6.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.15.230 0.0.0.1 10.6.150.0 0.0.0.255 eq www 443</t>
-        </is>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.150.0 0.0.0.255 eq www 443 10.6.15.230 0.0.0.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="294">
-      <c r="A294" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN80-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.80.0 0.0.0.15 10.6.86.0 0.0.0.255 eq 22 www 443 5480 5900 5601 8000 8980 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.80.0 0.0.0.15 host 10.6.88.243 eq 443 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.80.0 0.0.0.15 host 10.6.88.221 eq www 8888 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.80.0 0.0.0.15 10.6.88.0 0.0.0.255 eq ftp 22 telnet www 443 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN86-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.86.0 0.0.0.255 eq 22 www 443 5480 5900 5601 8000 8980 10.6.80.0 0.0.0.15 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="inlineStr">
-        <is>
-          <t>permit ip host 10.6.86.32 10.6.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="inlineStr">
-        <is>
-          <t>permit ip host 10.6.86.33 10.6.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="inlineStr">
-        <is>
-          <t>permit ip host 10.6.86.110 10.6.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="inlineStr">
-        <is>
-          <t>permit ip host 10.6.86.52 host 10.6.88.222</t>
-        </is>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="inlineStr">
-        <is>
-          <t>permit ip host 10.6.86.62 host 10.6.88.222</t>
-        </is>
-      </c>
-    </row>
-    <row r="308">
-      <c r="A308" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN88-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>permit udp host 10.6.88.222 host 10.6.88.254 eq snmp log</t>
-        </is>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" t="inlineStr">
-        <is>
-          <t>permit ip 10.6.88.0 0.0.0.255 host 10.6.86.32 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" t="inlineStr">
-        <is>
-          <t>permit ip 10.6.88.0 0.0.0.255 host 10.6.86.33 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" t="inlineStr">
-        <is>
-          <t>permit tcp 10.6.88.0 0.0.0.255 eq ftp 22 telnet www 443 10.6.80.0 0.0.0.15 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="313">
-      <c r="A313" t="inlineStr">
-        <is>
-          <t>permit ip 10.6.88.0 0.0.0.255 host 10.6.86.110 log</t>
         </is>
       </c>
     </row>
@@ -7188,7 +7040,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A213"/>
+  <dimension ref="A1:B191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7197,12 +7049,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX02-CS01-N9K-JPIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX02-CS01-N9K-JPIDC.log</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>20251129-HX02-OOB-DS01-C3850-JPIDC.log</t>
         </is>
       </c>
     </row>
@@ -7212,6 +7070,11 @@
           <t>ip access-list VLAN108-ACL</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN15-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7219,6 +7082,11 @@
           <t>52 permit tcp 10.12.108.0/24 10.12.62.11/32 eq 16000 log</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.12.150.244 eq 22 host 10.12.108.60</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7226,6 +7094,11 @@
           <t>60 permit tcp 10.12.108.0/24 10.12.62.66/32 eq www log</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.12.150.244 eq 443 host 10.12.62.32</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7233,6 +7106,11 @@
           <t>90 permit tcp 10.12.108.0/24 eq 55888 10.12.200.88/32 log</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>permit udp 10.12.15.0 0.0.0.255 eq snmp 10.12.62.8 0.0.0.7</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7240,6 +7118,11 @@
           <t>280 permit tcp 10.12.108.60/32 10.12.19.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>permit udp 10.12.150.0 0.0.0.255 eq snmp 10.12.62.8 0.0.0.7</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7247,6 +7130,11 @@
           <t>282 permit tcp 10.12.108.60/32 10.12.12.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>permit tcp 10.12.15.0 0.0.0.255 eq 443 5900 10.12.62.32 0.0.0.1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7254,6 +7142,11 @@
           <t>284 permit tcp 10.12.108.60/32 10.12.100.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>permit tcp 10.12.150.0 0.0.0.255 eq 443 5900 10.12.62.32 0.0.0.1</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7261,6 +7154,11 @@
           <t>286 permit tcp 10.12.108.60/32 10.12.0.0/16 eq 22</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.12.15.230 eq 3389 host 10.12.88.220</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7268,6 +7166,11 @@
           <t>288 permit icmp 10.12.108.60/32 10.12.0.0/16</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.12.15.243 eq 22 host 10.12.108.60</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7275,6 +7178,11 @@
           <t>290 permit tcp 10.12.108.60/32 10.12.76.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.12.15.244 eq 22 host 10.12.108.60</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -7282,6 +7190,11 @@
           <t>ip access-list VLAN168-ACL</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN153-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -7289,6 +7202,11 @@
           <t>52 permit tcp 10.12.168.0/24 10.12.62.11/32 eq 16000 log</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.12.153.1 eq 3389 host 10.12.88.200</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -7303,6 +7221,11 @@
           <t>222 permit tcp 10.12.168.24/30 10.12.169.0/30 range 8001 8004</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN88-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -7310,6 +7233,11 @@
           <t>224 permit tcp 10.12.168.20/30 10.12.169.0/30 eq 6788</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.12.88.220 10.12.88.0 0.0.0.255 eq 22</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -7317,6 +7245,11 @@
           <t>226 permit tcp 10.12.168.24/30 10.12.169.0/30 eq 6788</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>permit udp host 10.12.88.200 host 10.12.88.254 eq snmp</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -7324,6 +7257,11 @@
           <t>228 permit tcp 10.12.168.20/30 10.12.169.4/32 range 8001 8004</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>permit udp host 10.12.88.200 10.12.88.0 0.0.0.255 eq snmp</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -7331,6 +7269,11 @@
           <t>230 permit tcp 10.12.168.24/30 10.12.169.4/32 range 8001 8004</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>permit udp host 10.12.88.200 10.12.89.0 0.0.0.255 eq snmp</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -8477,132 +8420,6 @@
       <c r="A191" t="inlineStr">
         <is>
           <t>252 permit ip 10.12.8.43/32 10.12.17.0/24</t>
-        </is>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX02-OOB-DS01-C3850-JPIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN15-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.12.150.244 eq 22 host 10.12.108.60</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.12.150.244 eq 443 host 10.12.62.32</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>permit udp 10.12.15.0 0.0.0.255 eq snmp 10.12.62.8 0.0.0.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>permit udp 10.12.150.0 0.0.0.255 eq snmp 10.12.62.8 0.0.0.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>permit tcp 10.12.15.0 0.0.0.255 eq 443 5900 10.12.62.32 0.0.0.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>permit tcp 10.12.150.0 0.0.0.255 eq 443 5900 10.12.62.32 0.0.0.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.12.15.230 eq 3389 host 10.12.88.220</t>
-        </is>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.12.15.243 eq 22 host 10.12.108.60</t>
-        </is>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.12.15.244 eq 22 host 10.12.108.60</t>
-        </is>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN153-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.12.153.1 eq 3389 host 10.12.88.200</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN88-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.12.88.220 10.12.88.0 0.0.0.255 eq 22</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>permit udp host 10.12.88.200 host 10.12.88.254 eq snmp</t>
-        </is>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>permit udp host 10.12.88.200 10.12.88.0 0.0.0.255 eq snmp</t>
-        </is>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>permit udp host 10.12.88.200 10.12.89.0 0.0.0.255 eq snmp</t>
         </is>
       </c>
     </row>
@@ -8617,7 +8434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A127"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8626,12 +8443,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX03-CS01-N9K-JPIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX03-CS01-N9K-JPIDC.log</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>20251129-HX03-OOB-DS01-C3850-JPIDC.log</t>
         </is>
       </c>
     </row>
@@ -8641,6 +8464,11 @@
           <t>ip access-list VLAN108-ACL</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN15-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8648,6 +8476,11 @@
           <t>46 permit tcp 10.13.108.0/24 10.13.62.11/32 eq 16000 log</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>permit udp 10.13.15.0 0.0.0.255 eq snmp 10.13.62.8 0.0.0.7</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8655,6 +8488,11 @@
           <t>60 permit tcp 10.13.108.0/24 10.13.62.66/32 eq www log</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>permit udp 10.13.150.0 0.0.0.255 eq snmp 10.13.62.8 0.0.0.7</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8662,6 +8500,11 @@
           <t>280 permit tcp 10.13.108.60/32 10.13.19.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>permit tcp 10.13.15.0 0.0.0.255 eq 443 5900 10.13.62.32 0.0.0.1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8669,6 +8512,11 @@
           <t>282 permit tcp 10.13.108.60/32 10.13.12.0/24 eq 443</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>permit tcp 10.13.150.0 0.0.0.255 eq 443 5900 10.13.62.32 0.0.0.1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8676,6 +8524,11 @@
           <t>284 permit tcp 10.13.108.60/32 10.13.0.0/16 eq 22</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.13.15.243 eq 22 443 host 10.13.108.60</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8683,6 +8536,11 @@
           <t>286 permit icmp 10.13.108.60/32 10.13.0.0/16</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>permit tcp host 10.13.15.244 eq 22 host 10.13.108.60</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9395,62 +9253,6 @@
       <c r="A117" t="inlineStr">
         <is>
           <t>252 permit ip 10.13.8.43/32 10.13.17.0/24</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX03-OOB-DS01-C3850-JPIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN15-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>permit udp 10.13.15.0 0.0.0.255 eq snmp 10.13.62.8 0.0.0.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>permit udp 10.13.150.0 0.0.0.255 eq snmp 10.13.62.8 0.0.0.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>permit tcp 10.13.15.0 0.0.0.255 eq 443 5900 10.13.62.32 0.0.0.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>permit tcp 10.13.150.0 0.0.0.255 eq 443 5900 10.13.62.32 0.0.0.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.13.15.243 eq 22 443 host 10.13.108.60</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>permit tcp host 10.13.15.244 eq 22 host 10.13.108.60</t>
         </is>
       </c>
     </row>
@@ -9465,7 +9267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A702"/>
+  <dimension ref="A1:B646"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9474,12 +9276,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX04-CS01-N9K-JPIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX04-CS01-N9K-JPIDC.log</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>20251129-HX04-OOB-DS01-C9300-JPIDC.log</t>
         </is>
       </c>
     </row>
@@ -9489,6 +9297,11 @@
           <t>ip access-list VLAN100-ACL</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN150-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9496,6 +9309,11 @@
           <t>64 permit tcp 10.62.100.0/24 10.62.62.14/32 eq 16000</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.62.150.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9503,6 +9321,11 @@
           <t>162 permit tcp 10.62.100.96/29 eq 10081 10.62.106.18/31</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.62.150.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9510,6 +9333,11 @@
           <t>163 permit tcp 10.62.100.170/31 eq 10081 10.62.106.18/31</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>60 permit icmp 10.62.150.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9517,6 +9345,11 @@
           <t>248 permit tcp 10.62.100.0/24 10.62.110.0/24 eq 3399</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>70 permit tcp host 10.62.150.193 eq 22 host 10.62.108.60 log</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9524,6 +9357,11 @@
           <t>260 permit tcp 10.62.100.0/24 eq 55888 10.62.108.63/32</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>80 permit tcp host 10.62.150.194 eq 22 host 10.62.108.60 log</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9538,6 +9376,11 @@
           <t>272 permit tcp 10.62.100.96/28 range 19001 19002 10.62.16.0/30</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN151-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9545,6 +9388,11 @@
           <t>273 permit tcp 10.62.100.170/31 range 19001 19002 10.62.16.0/30</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.62.151.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -9552,6 +9400,11 @@
           <t>276 permit tcp 10.62.100.0/24 10.62.110.0/24 range 6633 6788</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.62.151.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -9559,6 +9412,11 @@
           <t>278 permit tcp 10.62.100.0/24 10.62.110.0/24 range 9092 9200</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>60 permit icmp 10.62.151.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -9573,6 +9431,11 @@
           <t>282 permit tcp 10.62.100.0/24 10.62.120.0/24 range 3366 3399</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN152-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -9580,6 +9443,11 @@
           <t>284 permit tcp 10.62.100.0/24 10.62.120.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.62.152.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -9587,6 +9455,11 @@
           <t>286 permit tcp 10.62.100.0/24 10.62.120.0/24 range 6633 6788</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.62.152.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -9594,6 +9467,11 @@
           <t>288 permit tcp 10.62.100.0/24 10.62.120.0/24 range 9092 9200</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>60 permit icmp 10.62.152.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -9608,6 +9486,11 @@
           <t>300 permit tcp 10.62.100.0/24 10.62.16.41/32 eq 8080</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN153-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -9615,6 +9498,11 @@
           <t>310 permit tcp 10.62.100.0/24 10.62.110.0/24 range 3366 3368</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.62.153.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -9622,6 +9510,11 @@
           <t>320 permit tcp 10.62.100.0/24 10.62.110.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.62.153.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -9629,6 +9522,11 @@
           <t>330 permit tcp 10.62.100.0/24 10.62.110.0/24 range 7001 7004</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>60 permit icmp 10.62.153.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -9643,6 +9541,11 @@
           <t>336 permit tcp 10.62.100.127/32 eq 50051 10.62.106.16/28</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN155-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -9650,6 +9553,11 @@
           <t>338 permit tcp 10.62.100.128/29 eq 50051 10.62.106.16/28</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.62.155.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -9657,6 +9565,11 @@
           <t>340 permit tcp 10.62.100.0/24 10.62.62.96/28 eq 9092</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.62.155.240 0.0.0.7 eq 443 host 10.62.62.32 log</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -9664,6 +9577,11 @@
           <t>350 permit tcp 10.62.100.0/24 10.62.130.0/24 range 3366 3368</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>60 permit tcp 10.62.155.240 0.0.0.7 host 10.62.200.60 eq 1000 log</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -9671,6 +9589,11 @@
           <t>352 permit tcp 10.62.100.0/24 10.62.130.0/24 range 7001 7004</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>70 permit icmp 10.62.155.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -9685,6 +9608,11 @@
           <t>356 permit tcp 10.62.100.0/24 10.62.130.0/24 eq 6633</t>
         </is>
       </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN86-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -9692,6 +9620,11 @@
           <t>358 permit tcp 10.62.100.0/24 10.62.130.0/24 eq 9092</t>
         </is>
       </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>70 permit ip host 10.62.86.2 host 10.62.88.251 log</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -9699,6 +9632,11 @@
           <t>360 permit tcp 10.62.100.0/24 10.60.110.0/24 eq 9200</t>
         </is>
       </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>80 permit udp host 10.62.86.2 10.60.88.0 0.0.0.255 log</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -9713,6 +9651,11 @@
           <t>370 permit tcp 10.62.100.0/26 range 17010 17040 10.62.106.32/27</t>
         </is>
       </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN88-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -9720,6 +9663,11 @@
           <t>372 permit tcp 10.62.100.64/27 range 17010 17040 10.62.106.32/27</t>
         </is>
       </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>120 permit ip 10.62.88.0 0.0.0.255 10.62.86.2 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -9741,6 +9689,11 @@
           <t>378 permit tcp 10.62.100.64/26 eq 17060 10.62.106.32/27</t>
         </is>
       </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>20251129-HX04-OOB-DS02-C9200L-JPIDC.log</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -9748,6 +9701,11 @@
           <t>380 permit tcp 10.62.100.64/26 range 20000 20020 10.62.106.32/27</t>
         </is>
       </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ip access-list extended F5_Mgmt_ACL</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -9755,6 +9713,11 @@
           <t>392 permit tcp 10.62.100.96/29 eq 8081 10.62.106.18/31</t>
         </is>
       </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>760 permit tcp 10.62.155.240 0.0.0.7 eq 443 host 10.62.62.32</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -9769,6 +9732,11 @@
           <t>394 permit tcp 10.62.100.64/26 eq 20000 10.62.106.18/31</t>
         </is>
       </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ip access-list extended Sec_ACL</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -9776,6 +9744,11 @@
           <t>398 permit tcp 10.62.100.0/24 10.62.130.233/32 eq 3366</t>
         </is>
       </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>280 permit tcp 10.60.15.192 0.0.0.63 eq 22 host 10.62.15.221 log</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -9783,6 +9756,11 @@
           <t>400 permit ip 10.62.100.0/25 10.62.106.8/29</t>
         </is>
       </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>300 permit udp 10.60.15.192 0.0.0.63 eq snmp host 10.62.15.198 log</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -9790,6 +9768,11 @@
           <t>422 permit tcp 10.62.100.96/29 eq 17998 10.62.106.16/30</t>
         </is>
       </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>720 permit tcp 10.60.150.0 0.0.0.255 eq www 443 10.62.62.32 0.0.0.7</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -9797,6 +9780,11 @@
           <t>423 permit tcp 10.62.100.170/31 eq 17998 10.62.106.16/30</t>
         </is>
       </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>730 permit tcp 10.60.150.0 0.0.0.255 eq 10050 10.60.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -9804,6 +9792,11 @@
           <t>428 permit tcp 10.62.100.40/29 eq 27040 10.62.106.16/31</t>
         </is>
       </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>740 permit tcp 10.60.150.0 0.0.0.255 10.60.62.8 0.0.0.7 eq 10051 log</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -9811,6 +9804,11 @@
           <t>430 permit tcp 10.62.100.64/26 eq 17060 10.62.106.16/31</t>
         </is>
       </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>750 permit udp 10.60.150.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -9818,6 +9816,11 @@
           <t>434 permit tcp 10.62.100.32/28 10.62.106.32/31 eq 9080</t>
         </is>
       </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>760 permit tcp 10.62.150.0 0.0.0.255 eq 443 5900 host 10.62.62.32</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -9832,6 +9835,11 @@
           <t>442 permit tcp 10.62.100.0/24 10.60.110.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN88-Mgmt</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -9839,6 +9847,11 @@
           <t>444 permit tcp 10.62.100.0/24 10.60.110.0/24 range 7001 7004</t>
         </is>
       </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>580 permit udp 10.60.88.192 0.0.0.63 host 10.62.88.221 eq syslog log</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -9846,6 +9859,11 @@
           <t>446 permit tcp 10.62.100.0/24 10.60.110.0/24 eq 9092</t>
         </is>
       </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>600 permit ip 10.60.88.0 0.0.0.255 10.62.80.96 0.0.0.31</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -9853,6 +9871,11 @@
           <t>456 permit tcp 10.62.100.0/24 10.60.110.0/24 range 6633 6788</t>
         </is>
       </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>640 permit ip 10.60.88.0 0.0.0.255 host 10.62.86.2 log</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -13663,9 +13686,9 @@
       </c>
     </row>
     <row r="614">
-      <c r="A614" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX04-CS03-N9K-JPIDC.log</t>
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>20251129-HX04-CS03-N9K-JPIDC.log</t>
         </is>
       </c>
     </row>
@@ -13890,314 +13913,6 @@
       <c r="A646" t="inlineStr">
         <is>
           <t>942 permit icmp 10.60.110.0/24 10.62.108.60/30</t>
-        </is>
-      </c>
-    </row>
-    <row r="649">
-      <c r="A649" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX04-OOB-DS01-C9300-JPIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="650">
-      <c r="A650" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN150-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="651">
-      <c r="A651" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.62.150.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="652">
-      <c r="A652" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.62.150.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="653">
-      <c r="A653" t="inlineStr">
-        <is>
-          <t>60 permit icmp 10.62.150.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="654">
-      <c r="A654" t="inlineStr">
-        <is>
-          <t>70 permit tcp host 10.62.150.193 eq 22 host 10.62.108.60 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="655">
-      <c r="A655" t="inlineStr">
-        <is>
-          <t>80 permit tcp host 10.62.150.194 eq 22 host 10.62.108.60 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="657">
-      <c r="A657" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN151-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="658">
-      <c r="A658" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.62.151.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="659">
-      <c r="A659" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.62.151.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="660">
-      <c r="A660" t="inlineStr">
-        <is>
-          <t>60 permit icmp 10.62.151.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="662">
-      <c r="A662" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN152-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="663">
-      <c r="A663" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.62.152.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="664">
-      <c r="A664" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.62.152.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="665">
-      <c r="A665" t="inlineStr">
-        <is>
-          <t>60 permit icmp 10.62.152.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="667">
-      <c r="A667" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN153-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="668">
-      <c r="A668" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.62.153.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="669">
-      <c r="A669" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.62.153.0 0.0.0.255 eq 443 5900 10.62.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="670">
-      <c r="A670" t="inlineStr">
-        <is>
-          <t>60 permit icmp 10.62.153.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="672">
-      <c r="A672" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN155-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="673">
-      <c r="A673" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.62.155.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="674">
-      <c r="A674" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.62.155.240 0.0.0.7 eq 443 host 10.62.62.32 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="675">
-      <c r="A675" t="inlineStr">
-        <is>
-          <t>60 permit tcp 10.62.155.240 0.0.0.7 host 10.62.200.60 eq 1000 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="676">
-      <c r="A676" t="inlineStr">
-        <is>
-          <t>70 permit icmp 10.62.155.0 0.0.0.255 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="678">
-      <c r="A678" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN86-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="679">
-      <c r="A679" t="inlineStr">
-        <is>
-          <t>70 permit ip host 10.62.86.2 host 10.62.88.251 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="680">
-      <c r="A680" t="inlineStr">
-        <is>
-          <t>80 permit udp host 10.62.86.2 10.60.88.0 0.0.0.255 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="682">
-      <c r="A682" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN88-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="683">
-      <c r="A683" t="inlineStr">
-        <is>
-          <t>120 permit ip 10.62.88.0 0.0.0.255 10.62.86.2 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="686">
-      <c r="A686" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX04-OOB-DS02-C9200L-JPIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="687">
-      <c r="A687" t="inlineStr">
-        <is>
-          <t>ip access-list extended F5_Mgmt_ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="688">
-      <c r="A688" t="inlineStr">
-        <is>
-          <t>760 permit tcp 10.62.155.240 0.0.0.7 eq 443 host 10.62.62.32</t>
-        </is>
-      </c>
-    </row>
-    <row r="690">
-      <c r="A690" t="inlineStr">
-        <is>
-          <t>ip access-list extended Sec_ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="691">
-      <c r="A691" t="inlineStr">
-        <is>
-          <t>280 permit tcp 10.60.15.192 0.0.0.63 eq 22 host 10.62.15.221 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="692">
-      <c r="A692" t="inlineStr">
-        <is>
-          <t>300 permit udp 10.60.15.192 0.0.0.63 eq snmp host 10.62.15.198 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="693">
-      <c r="A693" t="inlineStr">
-        <is>
-          <t>720 permit tcp 10.60.150.0 0.0.0.255 eq www 443 10.62.62.32 0.0.0.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="694">
-      <c r="A694" t="inlineStr">
-        <is>
-          <t>730 permit tcp 10.60.150.0 0.0.0.255 eq 10050 10.60.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="695">
-      <c r="A695" t="inlineStr">
-        <is>
-          <t>740 permit tcp 10.60.150.0 0.0.0.255 10.60.62.8 0.0.0.7 eq 10051 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="696">
-      <c r="A696" t="inlineStr">
-        <is>
-          <t>750 permit udp 10.60.150.0 0.0.0.255 eq snmp 10.62.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="697">
-      <c r="A697" t="inlineStr">
-        <is>
-          <t>760 permit tcp 10.62.150.0 0.0.0.255 eq 443 5900 host 10.62.62.32</t>
-        </is>
-      </c>
-    </row>
-    <row r="699">
-      <c r="A699" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN88-Mgmt</t>
-        </is>
-      </c>
-    </row>
-    <row r="700">
-      <c r="A700" t="inlineStr">
-        <is>
-          <t>580 permit udp 10.60.88.192 0.0.0.63 host 10.62.88.221 eq syslog log</t>
-        </is>
-      </c>
-    </row>
-    <row r="701">
-      <c r="A701" t="inlineStr">
-        <is>
-          <t>600 permit ip 10.60.88.0 0.0.0.255 10.62.80.96 0.0.0.31</t>
-        </is>
-      </c>
-    </row>
-    <row r="702">
-      <c r="A702" t="inlineStr">
-        <is>
-          <t>640 permit ip 10.60.88.0 0.0.0.255 host 10.62.86.2 log</t>
         </is>
       </c>
     </row>
@@ -14212,7 +13927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A616"/>
+  <dimension ref="A1:B591"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14221,12 +13936,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX05-CS01-N9K-JPIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX05-CS01-N9K-JPIDC.log</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>20251129-HX05-OOB-DS01-C9300-JPIDC.log</t>
         </is>
       </c>
     </row>
@@ -14236,6 +13957,11 @@
           <t>ip access-list VLAN100-ACL</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN150-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -14243,6 +13969,11 @@
           <t>2 permit tcp 10.65.100.196/30 eq 6443 10.65.170.8/32</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.65.150.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -14250,6 +13981,11 @@
           <t>68 permit tcp 10.65.100.0/24 10.65.62.11/32 eq 16000</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.65.150.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -14257,6 +13993,11 @@
           <t>162 permit ip 10.65.100.192/25 10.65.170.0/24</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>60 permit udp 10.65.15.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -14264,6 +14005,11 @@
           <t>258 permit tcp 10.65.100.0/24 10.65.120.0/24 eq 9201</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>70 permit tcp 10.65.15.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -14278,6 +14024,11 @@
           <t>264 permit tcp 10.65.100.0/24 10.65.110.0/24 range 3366 9200</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN151-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -14285,6 +14036,11 @@
           <t>266 permit tcp 10.65.100.0/24 10.65.120.0/24 range 3366 9200</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.65.151.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -14292,6 +14048,11 @@
           <t>268 permit tcp 10.65.100.0/24 10.65.16.53/32 eq domain</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.65.151.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -14306,6 +14067,11 @@
           <t>272 permit tcp 10.65.100.0/24 10.65.106.32/30 eq 8080</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN152-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -14313,6 +14079,11 @@
           <t>284 permit tcp 10.65.100.0/24 10.65.62.60/32 eq 1000</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.65.152.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -14320,6 +14091,11 @@
           <t>286 permit tcp 10.65.100.0/24 10.65.130.0/24 eq 6633</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.65.152.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -14334,6 +14110,11 @@
           <t>290 permit tcp 10.65.100.0/24 10.65.130.0/24 eq 3399</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN153-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -14341,6 +14122,11 @@
           <t>292 permit tcp 10.65.100.0/24 10.65.130.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.65.153.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -14348,6 +14134,11 @@
           <t>294 permit tcp 10.65.100.0/24 10.65.130.0/24 eq 9200</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.65.153.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -14362,6 +14153,11 @@
           <t>298 permit tcp 10.65.100.0/24 10.65.130.0/24 eq 9092</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN155-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -14369,6 +14165,11 @@
           <t>300 permit tcp 10.65.100.0/24 range 8081 20020 10.65.106.0/24</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.65.155.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -14376,6 +14177,11 @@
           <t>302 permit tcp 10.65.100.128/28 10.65.16.30/32 range 4000 4001</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.65.155.0 0.0.0.255 eq 22 host 10.65.108.60 log</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -14383,6 +14189,11 @@
           <t>310 permit tcp 10.65.100.0/24 eq 50051 10.65.106.0/24</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>60 permit tcp 10.65.155.0 0.0.0.255 eq 443 10.65.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -18266,139 +18077,6 @@
       <c r="A591" t="inlineStr">
         <is>
           <t>264 permit tcp 10.65.7.0/24 10.65.62.60/32 eq 1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="594">
-      <c r="A594" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX05-OOB-DS01-C9300-JPIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="595">
-      <c r="A595" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN150-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="596">
-      <c r="A596" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.65.150.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="597">
-      <c r="A597" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.65.150.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="598">
-      <c r="A598" t="inlineStr">
-        <is>
-          <t>60 permit udp 10.65.15.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="599">
-      <c r="A599" t="inlineStr">
-        <is>
-          <t>70 permit tcp 10.65.15.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="601">
-      <c r="A601" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN151-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="602">
-      <c r="A602" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.65.151.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="603">
-      <c r="A603" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.65.151.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="605">
-      <c r="A605" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN152-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="606">
-      <c r="A606" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.65.152.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="607">
-      <c r="A607" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.65.152.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="609">
-      <c r="A609" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN153-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="610">
-      <c r="A610" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.65.153.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="611">
-      <c r="A611" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.65.153.0 0.0.0.255 eq 443 5900 10.65.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="613">
-      <c r="A613" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN155-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="614">
-      <c r="A614" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.65.155.0 0.0.0.255 eq snmp 10.65.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="615">
-      <c r="A615" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.65.155.0 0.0.0.255 eq 22 host 10.65.108.60 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="616">
-      <c r="A616" t="inlineStr">
-        <is>
-          <t>60 permit tcp 10.65.155.0 0.0.0.255 eq 443 10.65.62.32 0.0.0.1 log</t>
         </is>
       </c>
     </row>
@@ -18413,7 +18091,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1502"/>
+  <dimension ref="A1:B1455"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18422,12 +18100,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX06-CS01-N9K-JPIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX06-CS01-N9K-JPIDC.log</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>20251129-HX06-OOB-DS01-C9300-JPIDC.log</t>
         </is>
       </c>
     </row>
@@ -18437,6 +18121,11 @@
           <t>ip access-list VLAN100-ACL</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN150-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -18444,6 +18133,11 @@
           <t>10 permit tcp 10.66.100.200/27 10.66.106.21/32 eq 10000</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.150.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -18451,6 +18145,11 @@
           <t>48 permit tcp 10.66.100.0/24 eq 22 10.66.108.60/32</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.150.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -18465,6 +18164,11 @@
           <t>66 permit tcp 10.66.100.0/24 eq 55888 10.66.108.65/32</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN151-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -18472,6 +18176,11 @@
           <t>124 permit tcp 10.66.100.0/24 10.66.62.11/32 eq 16000</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.151.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -18479,6 +18188,11 @@
           <t>162 permit ip 10.66.100.0/24 10.66.108.63/32</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.151.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -18493,6 +18207,11 @@
           <t>166 permit ip 10.66.100.0/24 10.66.16.0/24</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN152-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -18500,6 +18219,11 @@
           <t>168 permit tcp 10.66.100.215/32 eq www 10.66.62.88/31</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.152.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -18507,6 +18231,11 @@
           <t>170 permit tcp 10.66.100.215/32 eq 443 10.66.62.88/31</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.152.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -18521,6 +18250,11 @@
           <t>174 permit tcp 10.66.100.215/32 eq 443 10.66.62.88/32</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN153-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -18528,6 +18262,11 @@
           <t>176 permit tcp 10.66.100.215/32 eq www 10.66.62.89/32</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.153.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -18535,6 +18274,11 @@
           <t>178 permit tcp 10.66.100.215/32 eq 443 10.66.62.89/32</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.153.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -18549,6 +18293,11 @@
           <t>182 permit tcp 10.66.100.208/31 10.66.62.96/28 eq 9092</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN155-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -18556,6 +18305,11 @@
           <t>184 permit tcp 10.66.100.220/30 10.66.62.96/28 eq 9092</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.155.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -18563,6 +18317,11 @@
           <t>186 permit tcp 10.66.100.224/32 10.66.62.96/28 eq 9092</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.155.0 0.0.0.255 eq 443 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -18570,6 +18329,11 @@
           <t>188 permit tcp 10.66.100.0/24 10.66.106.49/30 eq 5432</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>60 permit tcp 10.66.155.0 0.0.0.255 eq 22 host 10.66.108.60 log</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -18584,6 +18348,11 @@
           <t>200 permit tcp 10.66.100.192/27 10.66.16.41/32 eq 8080</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN156-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -18591,6 +18360,11 @@
           <t>202 permit tcp 10.66.100.224/32 10.66.16.41/32 eq 8080</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.156.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -18598,6 +18372,11 @@
           <t>228 permit tcp 10.66.100.192/27 10.66.120.0/24 eq 9201</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.156.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -18605,6 +18384,11 @@
           <t>230 permit tcp 10.66.100.192/27 10.66.110.0/24 range 6633 6788</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>60 permit tcp 10.66.156.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -18619,6 +18403,11 @@
           <t>234 permit tcp 10.66.100.192/27 10.66.110.0/24 range 9091 9200</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN157-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -18626,6 +18415,11 @@
           <t>236 permit tcp 10.66.100.224/32 10.66.110.0/24 range 9091 9200</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.157.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -18633,6 +18427,11 @@
           <t>238 permit tcp 10.66.100.192/27 10.66.110.0/24 range 7001 7004</t>
         </is>
       </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.157.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -18640,6 +18439,11 @@
           <t>240 permit tcp 10.66.100.224/32 10.66.110.0/24 range 7001 7004</t>
         </is>
       </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>60 permit tcp 10.66.157.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -18654,6 +18458,11 @@
           <t>244 permit tcp 10.66.100.224/32 10.66.110.0/24 range 3366 3399</t>
         </is>
       </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN158-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -18661,6 +18470,11 @@
           <t>246 permit tcp 10.66.100.192/27 10.66.110.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.158.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -18668,6 +18482,11 @@
           <t>248 permit tcp 10.66.100.224/32 10.66.110.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.158.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -18675,6 +18494,11 @@
           <t>250 permit tcp 10.66.100.192/27 10.66.120.0/24 range 6633 6788</t>
         </is>
       </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>60 permit tcp 10.66.158.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -18689,6 +18513,11 @@
           <t>254 permit tcp 10.66.100.192/27 10.66.120.0/24 range 9091 9200</t>
         </is>
       </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN159-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -18696,6 +18525,11 @@
           <t>256 permit tcp 10.66.100.224/32 10.66.120.0/24 range 9091 9200</t>
         </is>
       </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>40 permit udp 10.66.159.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -18703,6 +18537,11 @@
           <t>258 permit tcp 10.66.100.192/27 10.66.120.0/24 range 7001 7004</t>
         </is>
       </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>50 permit tcp 10.66.159.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -18710,6 +18549,11 @@
           <t>260 permit tcp 10.66.100.224/32 10.66.120.0/24 range 7001 7004</t>
         </is>
       </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>60 permit tcp 10.66.159.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -18724,6 +18568,11 @@
           <t>264 permit tcp 10.66.100.224/32 10.66.120.0/24 range 3366 3399</t>
         </is>
       </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ip access-list extended VLAN88-ACL</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -18731,6 +18580,11 @@
           <t>266 permit tcp 10.66.100.192/27 10.66.120.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>120 permit ip host 10.66.88.211 host 10.66.62.33 log</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -18738,6 +18592,11 @@
           <t>268 permit tcp 10.66.100.224/32 10.66.120.0/24 eq 4000</t>
         </is>
       </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>130 permit ip host 10.66.88.212 host 10.66.62.33 log</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -25026,9 +24885,9 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX06-CS03-N9K-JPIDC.log</t>
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>20251129-HX06-CS03-N9K-JPIDC.log</t>
         </is>
       </c>
     </row>
@@ -28417,258 +28276,6 @@
       <c r="A1455" t="inlineStr">
         <is>
           <t>168 permit tcp 10.66.243.0/29 eq 4000 10.66.242.141/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="1458">
-      <c r="A1458" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX06-OOB-DS01-C9300-JPIDC.log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1459">
-      <c r="A1459" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN150-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1460">
-      <c r="A1460" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.150.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1461">
-      <c r="A1461" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.150.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1463">
-      <c r="A1463" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN151-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1464">
-      <c r="A1464" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.151.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1465">
-      <c r="A1465" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.151.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1467">
-      <c r="A1467" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN152-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1468">
-      <c r="A1468" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.152.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1469">
-      <c r="A1469" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.152.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1471">
-      <c r="A1471" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN153-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1472">
-      <c r="A1472" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.153.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1473">
-      <c r="A1473" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.153.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1475">
-      <c r="A1475" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN155-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1476">
-      <c r="A1476" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.155.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1477">
-      <c r="A1477" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.155.0 0.0.0.255 eq 443 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1478">
-      <c r="A1478" t="inlineStr">
-        <is>
-          <t>60 permit tcp 10.66.155.0 0.0.0.255 eq 22 host 10.66.108.60 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1480">
-      <c r="A1480" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN156-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1481">
-      <c r="A1481" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.156.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1482">
-      <c r="A1482" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.156.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1483">
-      <c r="A1483" t="inlineStr">
-        <is>
-          <t>60 permit tcp 10.66.156.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1485">
-      <c r="A1485" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN157-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1486">
-      <c r="A1486" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.157.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1487">
-      <c r="A1487" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.157.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1488">
-      <c r="A1488" t="inlineStr">
-        <is>
-          <t>60 permit tcp 10.66.157.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1490">
-      <c r="A1490" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN158-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1491">
-      <c r="A1491" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.158.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1492">
-      <c r="A1492" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.158.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1493">
-      <c r="A1493" t="inlineStr">
-        <is>
-          <t>60 permit tcp 10.66.158.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1495">
-      <c r="A1495" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN159-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1496">
-      <c r="A1496" t="inlineStr">
-        <is>
-          <t>40 permit udp 10.66.159.0 0.0.0.255 eq snmp 10.66.62.8 0.0.0.7 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1497">
-      <c r="A1497" t="inlineStr">
-        <is>
-          <t>50 permit tcp 10.66.159.0 0.0.0.255 eq 443 5900 10.66.62.32 0.0.0.1 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1498">
-      <c r="A1498" t="inlineStr">
-        <is>
-          <t>60 permit tcp 10.66.159.0 0.0.0.255 eq 443 5900 host 10.66.221.33 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1500">
-      <c r="A1500" t="inlineStr">
-        <is>
-          <t>ip access-list extended VLAN88-ACL</t>
-        </is>
-      </c>
-    </row>
-    <row r="1501">
-      <c r="A1501" t="inlineStr">
-        <is>
-          <t>120 permit ip host 10.66.88.211 host 10.66.62.33 log</t>
-        </is>
-      </c>
-    </row>
-    <row r="1502">
-      <c r="A1502" t="inlineStr">
-        <is>
-          <t>130 permit ip host 10.66.88.212 host 10.66.62.33 log</t>
         </is>
       </c>
     </row>
@@ -28692,12 +28299,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="120" customWidth="1" min="1" max="1"/>
+    <col width="120" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t># 设备: 20251129-HX11-CS01-N9K-JPIDC.log</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>20251129-HX11-CS01-N9K-JPIDC.log</t>
         </is>
       </c>
     </row>

</xml_diff>